<commit_message>
Refactored to address suggestion given in comments
</commit_message>
<xml_diff>
--- a/test_resource/codeextractor_T_T_A_D.xlsx
+++ b/test_resource/codeextractor_T_T_A_D.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="codeextractor" sheetId="1" r:id="rId1"/>
+    <sheet name="expeccodeextractor_T_T_A_D" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -34,56 +34,60 @@
     <t>CerberusTest.java_4</t>
   </si>
   <si>
-    <t xml:space="preserve">    }
-    @ After
-    public void afterAll() {
-        super.restoreStreams();
-    }
-    @Test
-    public void testCerebruswithOutArguments() {
-        Cerberus.main(new String[] {});
-        String expectedOutputString = getCerberusCommandLineUsageString();
-        assertEquals(expectedOutputString, getModifiedOutputStream().toString());
-    }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    public void testCerebruswithOutArguments() {
-        Cerberus.main(new String[] {});
-        String expectedOutputString = getCerberusCommandLineUsageString();
-        assertEquals(expectedOutputString, getModifiedOutputStream().toString());
-    }
-    @Test
-    public void testCerebrusWithArguments() {
-        getOriginalOutputStream().flush();
-        Cerberus.main(new String[] { "CPD" });
-    }
-    @Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    @Test
-    public void testCerebrusWithArguments() {
-        getOriginalOutputStream().flush();
-        Cerberus.main(new String[] { "CPD" });
-    }
-    @Test
-    public void testCerebruswithWrongArguments() {
-        String dummyArgument = "dummy argument";
-        Cerberus.main(new String[] { dummyArgument });
-        String expectedOutputString = new StringBuilder().append("Unmatched argument at index 0: 'dummy argument'").append(NEW_LINE).append(getCerberusCommandLineUsageString()).toString();
-    }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    public void testCerebruswithWrongArguments() {
-        String dummyArgument = "dummy argument";
-        Cerberus.main(new String[] { dummyArgument });
-        String expectedOutputString = new StringBuilder().append("Unmatched argument at index 0: 'dummy argument'").append(NEW_LINE).append(getCerberusCommandLineUsageString()).toString();
-    }
-    @Test
-    public void testCallMethod() throws Exception {
-        assertEquals(Integer.valueOf(0), new Cerberus().call());
-    }
-    private String getCerberusCommandLineUsageString() {
-        return new StringBuilder().append("Usage: Cerberus [COMMAND]").append(NEW_LINE).append("Waking Cerberus to devour bad things in the system").append(NEW_LINE).append("Commands:")</t>
+    <t xml:space="preserve">}_x000D_
+@ After_x000D_
+public void afterAll() {_x000D_
+super.restoreStreams()_x000D_
+}_x000D_
+@Test_x000D_
+public void testCerebruswithOutArguments() {_x000D_
+Cerberus.main(new String[] {})_x000D_
+String expectedOutputString = getCerberusCommandLineUsageString()_x000D_
+assertEquals(expectedOutputString, getModifiedOutputStream().toString())_x000D_
+}_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">public void testCerebruswithOutArguments() {_x000D_
+Cerberus.main(new String[] {})_x000D_
+String expectedOutputString = getCerberusCommandLineUsageString()_x000D_
+assertEquals(expectedOutputString, getModifiedOutputStream().toString())_x000D_
+}_x000D_
+@Test_x000D_
+public void testCerebrusWithArguments() {_x000D_
+getOriginalOutputStream().flush()_x000D_
+Cerberus.main(new String[] { "CPD" })_x000D_
+}_x000D_
+@Test_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Test_x000D_
+public void testCerebrusWithArguments() {_x000D_
+getOriginalOutputStream().flush()_x000D_
+Cerberus.main(new String[] { "CPD" })_x000D_
+}_x000D_
+@Test_x000D_
+public void testCerebruswithWrongArguments() {_x000D_
+String dummyArgument = "dummy argument"_x000D_
+Cerberus.main(new String[] { dummyArgument })_x000D_
+String expectedOutputString = new StringBuilder().append("Unmatched argument at index 0: 'dummy argument'").append(NEW_LINE).append(getCerberusCommandLineUsageString()).toString()_x000D_
+}_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">public void testCerebruswithWrongArguments() {_x000D_
+String dummyArgument = "dummy argument"_x000D_
+Cerberus.main(new String[] { dummyArgument })_x000D_
+String expectedOutputString = new StringBuilder().append("Unmatched argument at index 0: 'dummy argument'").append(NEW_LINE).append(getCerberusCommandLineUsageString()).toString()_x000D_
+}_x000D_
+@Test_x000D_
+public void testCallMethod() throws Exception {_x000D_
+assertEquals(Integer.valueOf(0), new Cerberus().call())_x000D_
+}_x000D_
+private String getCerberusCommandLineUsageString() {_x000D_
+return new StringBuilder().append("Usage: Cerberus [COMMAND]").append(NEW_LINE).append("Waking Cerberus to devour bad things in the system").append(NEW_LINE).append("Commands:")_x000D_
+</t>
   </si>
 </sst>
 </file>

</xml_diff>